<commit_message>
chart: fix issue with chart title formula font
Fix issue where the font change for a chart title that used a
formula wasn't set if the formatting was also set.
</commit_message>
<xml_diff>
--- a/tests/input/bootstrap64.xlsx
+++ b/tests/input/bootstrap64.xlsx
@@ -82,6 +82,20 @@
           </a:solidFill>
         </a:ln>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -172,24 +186,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="67991424"/>
-        <c:axId val="68001152"/>
+        <c:axId val="46566016"/>
+        <c:axId val="46842624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67991424"/>
+        <c:axId val="46566016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68001152"/>
+        <c:crossAx val="46842624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68001152"/>
+        <c:axId val="46842624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -197,7 +211,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67991424"/>
+        <c:crossAx val="46566016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -210,7 +224,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>